<commit_message>
SMART_RADAR_WEBAPP.V1.1.5-ALPHA - update benchmark - add org_email - fixed bug dashboard
</commit_message>
<xml_diff>
--- a/see-kpi-portlet/docroot/file/appraisal_organization_template.xlsx
+++ b/see-kpi-portlet/docroot/file/appraisal_organization_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GJ-Chokanan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toto\git\see-kpi-portlet-ghb\see-kpi-portlet\docroot\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F37C60B4-26E7-4E35-92AA-84E80373F268}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>org_code</t>
   </si>
@@ -42,12 +43,15 @@
   </si>
   <si>
     <t>longitude</t>
+  </si>
+  <si>
+    <t>org_email</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -415,22 +419,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="6" customWidth="1"/>
     <col min="2" max="3" width="25.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="16.140625" style="1"/>
+    <col min="4" max="5" width="15.28515625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="16.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1">
+    <row r="1" spans="1:7" s="3" customFormat="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -443,15 +447,18 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="lzkdQaDeirnBdT54UhH1rsujEQAwp4XEBoC/1MlVpW8n9gtmtNp8dJAiUYbNLpBV9zmzcjyhyAUcHIn5h/dRkw==" saltValue="juCknGux4F88YEOGVcWl6Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection deleteColumns="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>